<commit_message>
fix: installato googleapis per Drive
</commit_message>
<xml_diff>
--- a/data/exporters.xlsx
+++ b/data/exporters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luiss-my.sharepoint.com/personal/gianluca_palomba_studenti_luiss_it/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{468E9C45-602F-EC42-890D-92D473A3FC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E348E618-975A-7E49-A772-6E1B5DA930B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="3" xr2:uid="{5EAC376A-3442-1B45-B0D2-09E92A083557}"/>
   </bookViews>
@@ -122,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -130,8 +130,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +452,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0695C8EE-A3CD-7C4B-AE04-D4AD4E62590F}" name="Table5" displayName="Table5" ref="A1:D87" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:D87" xr:uid="{0695C8EE-A3CD-7C4B-AE04-D4AD4E62590F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0695C8EE-A3CD-7C4B-AE04-D4AD4E62590F}" name="Table5" displayName="Table5" ref="A1:D88" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:D88" xr:uid="{0695C8EE-A3CD-7C4B-AE04-D4AD4E62590F}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{8563848E-2A9A-B84A-A963-4734F1DF8550}" name="Week Number">
       <calculatedColumnFormula>WEEKNUM(Table5[[#This Row],[Week]])</calculatedColumnFormula>
@@ -469,8 +467,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC06151D-0F35-7F4F-B001-D163D9499F03}" name="Table52" displayName="Table52" ref="A1:D87" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A1:D87" xr:uid="{FC06151D-0F35-7F4F-B001-D163D9499F03}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC06151D-0F35-7F4F-B001-D163D9499F03}" name="Table52" displayName="Table52" ref="A1:D88" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A1:D88" xr:uid="{FC06151D-0F35-7F4F-B001-D163D9499F03}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{682CFEF3-7FE2-E64A-9BE5-FEBBFC2AD5DE}" name="Week Number"/>
     <tableColumn id="1" xr3:uid="{66DA498C-C289-5D43-B34E-A646ECFC68CE}" name="Week" dataDxfId="12"/>
@@ -484,8 +482,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB648CE3-B1C6-9642-8802-C6E40BAB18F1}" name="Table53" displayName="Table53" ref="A1:D87" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:D87" xr:uid="{EB648CE3-B1C6-9642-8802-C6E40BAB18F1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB648CE3-B1C6-9642-8802-C6E40BAB18F1}" name="Table53" displayName="Table53" ref="A1:D88" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:D88" xr:uid="{EB648CE3-B1C6-9642-8802-C6E40BAB18F1}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{11E1F86A-CCA6-7C4F-B54C-2BD7324A617A}" name="Week Number" dataDxfId="8"/>
     <tableColumn id="1" xr3:uid="{ACFCA92D-A205-FE41-9DA2-240C077A5066}" name="Week" dataDxfId="7"/>
@@ -499,8 +497,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42547EA6-FD94-D345-B399-847DD66C58F9}" name="Table54" displayName="Table54" ref="A1:D87" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D87" xr:uid="{42547EA6-FD94-D345-B399-847DD66C58F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42547EA6-FD94-D345-B399-847DD66C58F9}" name="Table54" displayName="Table54" ref="A1:D88" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D88" xr:uid="{42547EA6-FD94-D345-B399-847DD66C58F9}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{FC9E379E-9E93-984F-9ABD-A635D5E306F3}" name="Week Number" dataDxfId="3">
       <calculatedColumnFormula>WEEKNUM(Table54[[#This Row],[Week]])</calculatedColumnFormula>
@@ -832,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89D5D4B-46CB-C946-B5CE-C38558A8D632}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79:D87"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2083,7 +2081,7 @@
         <v>13</v>
       </c>
       <c r="B74" s="6">
-        <f t="shared" ref="B74:B87" si="9">B73+IF(WEEKDAY(B73+1)=1,2,1)</f>
+        <f t="shared" ref="B74:B88" si="9">B73+IF(WEEKDAY(B73+1)=1,2,1)</f>
         <v>45740</v>
       </c>
       <c r="C74" s="2">
@@ -2313,6 +2311,23 @@
       <c r="D87" s="2">
         <f>Table5[[#This Row],[Price]]-C86</f>
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f>WEEKNUM(Table5[[#This Row],[Week]])</f>
+        <v>15</v>
+      </c>
+      <c r="B88" s="6">
+        <f t="shared" si="9"/>
+        <v>45756</v>
+      </c>
+      <c r="C88" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="D88" s="2">
+        <f>Table5[[#This Row],[Price]]-C87</f>
+        <v>0.29999999999999982</v>
       </c>
     </row>
   </sheetData>
@@ -2325,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76C3511-ACE1-484A-B5B7-1ACF5FC5A911}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79:D87"/>
+      <selection activeCell="A87" sqref="A87:D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3574,7 +3589,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="3">
-        <f t="shared" ref="B70:B87" si="1">B69 + IF(WEEKDAY(B69) = 7, 2, 1)</f>
+        <f t="shared" ref="B70:B88" si="1">B69 + IF(WEEKDAY(B69) = 7, 2, 1)</f>
         <v>45735</v>
       </c>
       <c r="C70" s="4">
@@ -3757,7 +3772,7 @@
         <f t="shared" si="1"/>
         <v>45747</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="2">
         <f>ROUND('43LB 22XU'!C80 * (44 / 43), 1)</f>
         <v>6.7</v>
       </c>
@@ -3775,7 +3790,7 @@
         <f t="shared" si="1"/>
         <v>45748</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="2">
         <f>ROUND('43LB 22XU'!C81 * (44 / 43), 1)</f>
         <v>6.7</v>
       </c>
@@ -3793,7 +3808,7 @@
         <f t="shared" si="1"/>
         <v>45749</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="2">
         <f>ROUND('43LB 22XU'!C82 * (44 / 43), 1)</f>
         <v>6.7</v>
       </c>
@@ -3811,7 +3826,7 @@
         <f t="shared" si="1"/>
         <v>45750</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="2">
         <f>ROUND('43LB 22XU'!C83 * (44 / 43), 1)</f>
         <v>6.9</v>
       </c>
@@ -3829,7 +3844,7 @@
         <f t="shared" si="1"/>
         <v>45751</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="2">
         <f>ROUND('43LB 22XU'!C84 * (44 / 43), 1)</f>
         <v>6.7</v>
       </c>
@@ -3847,7 +3862,7 @@
         <f t="shared" si="1"/>
         <v>45752</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="2">
         <f>ROUND('43LB 22XU'!C85 * (44 / 43), 1)</f>
         <v>6.7</v>
       </c>
@@ -3865,7 +3880,7 @@
         <f t="shared" si="1"/>
         <v>45754</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="2">
         <f>ROUND('43LB 22XU'!C86 * (44 / 43), 1)</f>
         <v>6.9</v>
       </c>
@@ -3883,13 +3898,31 @@
         <f t="shared" si="1"/>
         <v>45755</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="2">
         <f>ROUND('43LB 22XU'!C87 * (44 / 43), 1)</f>
         <v>7.4</v>
       </c>
       <c r="D87" s="2">
         <f>Table52[[#This Row],[Price]]-C86</f>
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f>WEEKNUM(Table52[[#This Row],[Week]])</f>
+        <v>15</v>
+      </c>
+      <c r="B88" s="3">
+        <f t="shared" si="1"/>
+        <v>45756</v>
+      </c>
+      <c r="C88" s="2">
+        <f>ROUND('43LB 22XU'!C88 * (44 / 43), 1)</f>
+        <v>7.7</v>
+      </c>
+      <c r="D88" s="2">
+        <f>Table52[[#This Row],[Price]]-C87</f>
+        <v>0.29999999999999982</v>
       </c>
     </row>
   </sheetData>
@@ -3902,10 +3935,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770F52D7-1C6E-2A45-ACD5-A965EA26C2A8}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79:D87"/>
+      <selection activeCell="A87" sqref="A87:D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5152,7 +5185,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="3">
-        <f t="shared" ref="B70:B87" si="1">B69+IF(WEEKDAY(B69)=7,2,1)</f>
+        <f t="shared" ref="B70:B88" si="1">B69+IF(WEEKDAY(B69)=7,2,1)</f>
         <v>45735</v>
       </c>
       <c r="C70" s="4">
@@ -5335,7 +5368,7 @@
         <f t="shared" si="1"/>
         <v>45747</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="2">
         <f>ROUND('43LB 22XU'!C80 * (50 / 43), 1)</f>
         <v>7.6</v>
       </c>
@@ -5353,7 +5386,7 @@
         <f t="shared" si="1"/>
         <v>45748</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="2">
         <f>ROUND('43LB 22XU'!C81 * (50 / 43), 1)</f>
         <v>7.6</v>
       </c>
@@ -5371,7 +5404,7 @@
         <f t="shared" si="1"/>
         <v>45749</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="2">
         <f>ROUND('43LB 22XU'!C82 * (50 / 43), 1)</f>
         <v>7.6</v>
       </c>
@@ -5389,7 +5422,7 @@
         <f t="shared" si="1"/>
         <v>45750</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="2">
         <f>ROUND('43LB 22XU'!C83 * (50 / 43), 1)</f>
         <v>7.8</v>
       </c>
@@ -5407,7 +5440,7 @@
         <f t="shared" si="1"/>
         <v>45751</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="2">
         <f>ROUND('43LB 22XU'!C84 * (50 / 43), 1)</f>
         <v>7.6</v>
       </c>
@@ -5425,7 +5458,7 @@
         <f t="shared" si="1"/>
         <v>45752</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="2">
         <f>ROUND('43LB 22XU'!C85 * (50 / 43), 1)</f>
         <v>7.6</v>
       </c>
@@ -5443,7 +5476,7 @@
         <f t="shared" si="1"/>
         <v>45754</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="2">
         <f>ROUND('43LB 22XU'!C86 * (50 / 43), 1)</f>
         <v>7.8</v>
       </c>
@@ -5461,13 +5494,31 @@
         <f t="shared" si="1"/>
         <v>45755</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="2">
         <f>ROUND('43LB 22XU'!C87 * (50 / 43), 1)</f>
         <v>8.4</v>
       </c>
       <c r="D87" s="4">
         <f>Table53[[#This Row],[Price]]-C86</f>
         <v>0.60000000000000053</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <f>WEEKNUM(Table53[[#This Row],[Week]])</f>
+        <v>15</v>
+      </c>
+      <c r="B88" s="3">
+        <f t="shared" si="1"/>
+        <v>45756</v>
+      </c>
+      <c r="C88" s="2">
+        <f>ROUND('43LB 22XU'!C88 * (50 / 43), 1)</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D88" s="4">
+        <f>Table53[[#This Row],[Price]]-C87</f>
+        <v>0.29999999999999893</v>
       </c>
     </row>
   </sheetData>
@@ -5480,10 +5531,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA10450-6A51-F643-A4BD-9C5F01852BA0}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+      <selection activeCell="A87" sqref="A87:D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6729,7 +6780,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="3">
-        <f t="shared" ref="B70:B87" si="1">B69 + IF(WEEKDAY(B69) = 7, 2, 1)</f>
+        <f t="shared" ref="B70:B88" si="1">B69 + IF(WEEKDAY(B69) = 7, 2, 1)</f>
         <v>45735</v>
       </c>
       <c r="C70" s="4">
@@ -6904,7 +6955,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="8">
+      <c r="A80">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -6912,7 +6963,7 @@
         <f t="shared" si="1"/>
         <v>45747</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="2">
         <f>ROUND('43LB 22XU'!C80 * (31.5 / 43), 1)</f>
         <v>4.8</v>
       </c>
@@ -6922,7 +6973,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="8">
+      <c r="A81">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -6930,7 +6981,7 @@
         <f t="shared" si="1"/>
         <v>45748</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="2">
         <f>ROUND('43LB 22XU'!C81 * (31.5 / 43), 1)</f>
         <v>4.8</v>
       </c>
@@ -6940,7 +6991,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="8">
+      <c r="A82">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -6948,7 +6999,7 @@
         <f t="shared" si="1"/>
         <v>45749</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="2">
         <f>ROUND('43LB 22XU'!C82 * (31.5 / 43), 1)</f>
         <v>4.8</v>
       </c>
@@ -6958,7 +7009,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="8">
+      <c r="A83">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -6966,7 +7017,7 @@
         <f t="shared" si="1"/>
         <v>45750</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="2">
         <f>ROUND('43LB 22XU'!C83 * (31.5 / 43), 1)</f>
         <v>4.9000000000000004</v>
       </c>
@@ -6976,7 +7027,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="8">
+      <c r="A84">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -6984,7 +7035,7 @@
         <f t="shared" si="1"/>
         <v>45751</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="2">
         <f>ROUND('43LB 22XU'!C84 * (31.5 / 43), 1)</f>
         <v>4.8</v>
       </c>
@@ -6994,7 +7045,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="8">
+      <c r="A85">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>14</v>
       </c>
@@ -7002,7 +7053,7 @@
         <f t="shared" si="1"/>
         <v>45752</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="2">
         <f>ROUND('43LB 22XU'!C85 * (31.5 / 43), 1)</f>
         <v>4.8</v>
       </c>
@@ -7012,7 +7063,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="8">
+      <c r="A86">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>15</v>
       </c>
@@ -7020,7 +7071,7 @@
         <f t="shared" si="1"/>
         <v>45754</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="2">
         <f>ROUND('43LB 22XU'!C86 * (31.5 / 43), 1)</f>
         <v>4.9000000000000004</v>
       </c>
@@ -7030,7 +7081,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="8">
+      <c r="A87">
         <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
         <v>15</v>
       </c>
@@ -7038,13 +7089,31 @@
         <f t="shared" si="1"/>
         <v>45755</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="2">
         <f>ROUND('43LB 22XU'!C87 * (31.5 / 43), 1)</f>
         <v>5.3</v>
       </c>
       <c r="D87" s="2">
         <f>Table54[[#This Row],[Price]]-C86</f>
         <v>0.39999999999999947</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f>WEEKNUM(Table54[[#This Row],[Week]])</f>
+        <v>15</v>
+      </c>
+      <c r="B88" s="3">
+        <f t="shared" si="1"/>
+        <v>45756</v>
+      </c>
+      <c r="C88" s="2">
+        <f>ROUND('43LB 22XU'!C88 * (31.5 / 43), 1)</f>
+        <v>5.5</v>
+      </c>
+      <c r="D88" s="2">
+        <f>Table54[[#This Row],[Price]]-C87</f>
+        <v>0.20000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>